<commit_message>
Fix on metabolites of BIT
</commit_message>
<xml_diff>
--- a/Results/quality_metrics_compounds.xlsx
+++ b/Results/quality_metrics_compounds.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -587,6 +587,34 @@
         <v>0.9559859154929577</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>merlin_bit</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>720</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3506</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3357</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.1703738760056791</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.1766004415011038</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.1734312898952186</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.9305622528691291</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>